<commit_message>
gskau_template change +  changing seed and functional tests
</commit_message>
<xml_diff>
--- a/Projects/GSKAU/Data/gsk_set_up.xlsx
+++ b/Projects/GSKAU/Data/gsk_set_up.xlsx
@@ -14,7 +14,7 @@
     <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
-    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[2]Set_up!$A$90:$A$124</definedName>
+    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[1]Set_up!$A$90:$A$124</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Functional KPIs'!$A$1:$J$3</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -74,7 +74,7 @@
     <t xml:space="preserve">Exclude</t>
   </si>
   <si>
-    <t xml:space="preserve">Adult,Child,Denture,NRT,Toothpaste,Topical,Osteo</t>
+    <t xml:space="preserve">Adult,Child,Denture,NRT,Toothpaste,Topical,Osteo,Pain Other,Respiratory Other</t>
   </si>
   <si>
     <t xml:space="preserve">Availability</t>
@@ -232,6 +232,10 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -242,10 +246,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -324,7 +324,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </externalLink>
@@ -338,24 +338,24 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E20" activeCellId="0" sqref="E20"/>
+      <selection pane="bottomRight" activeCell="K3" activeCellId="0" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.2105263157895"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="29.5668016194332"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.3157894736842"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="1" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="29.1376518218623"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1014" min="13" style="1" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="1025" min="1015" style="0" width="8.67611336032389"/>
@@ -407,44 +407,44 @@
       <c r="C2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9" t="s">
+      <c r="D2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="9"/>
+      <c r="L2" s="10"/>
     </row>
     <row r="3" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="5"/>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="7" t="s">
+      <c r="E3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>14</v>
       </c>
       <c r="H3" s="0"/>
@@ -459,23 +459,23 @@
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
include others for sos
</commit_message>
<xml_diff>
--- a/Projects/GSKAU/Data/gsk_set_up.xlsx
+++ b/Projects/GSKAU/Data/gsk_set_up.xlsx
@@ -14,7 +14,7 @@
     <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
-    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[1]Set_up!$A$90:$A$124</definedName>
+    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[2]Set_up!$A$90:$A$124</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Functional KPIs'!$A$1:$J$3</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -74,6 +74,9 @@
     <t xml:space="preserve">Exclude</t>
   </si>
   <si>
+    <t xml:space="preserve">Include</t>
+  </si>
+  <si>
     <t xml:space="preserve">Adult,Child,Denture,NRT,Toothpaste,Topical,Osteo,Pain Other,Respiratory Other</t>
   </si>
   <si>
@@ -84,9 +87,6 @@
   </si>
   <si>
     <t xml:space="preserve">Linear SOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Include</t>
   </si>
 </sst>
 </file>
@@ -96,7 +96,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -133,12 +133,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -203,7 +197,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -230,10 +224,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -324,7 +314,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </externalLink>
@@ -338,24 +328,24 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K3" activeCellId="0" sqref="K3"/>
+      <selection pane="bottomRight" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.3157894736842"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="29.7773279352227"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.5303643724696"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="1" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="29.3522267206478"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1014" min="13" style="1" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="1025" min="1015" style="0" width="8.67611336032389"/>
@@ -407,75 +397,75 @@
       <c r="C2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="10" t="s">
+      <c r="D2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="10"/>
+      <c r="F2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" s="5"/>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="8" t="s">
+      <c r="D3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>14</v>
       </c>
       <c r="H3" s="0"/>
       <c r="I3" s="0"/>
       <c r="J3" s="0"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
+      <c r="D4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
PROS-11827-additional Main Shelf task wadded to SOS and Availability KPI
</commit_message>
<xml_diff>
--- a/Projects/GSKAU/Data/gsk_set_up.xlsx
+++ b/Projects/GSKAU/Data/gsk_set_up.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Functional KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,7 +14,7 @@
     <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
-    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[2]Set_up!$A$90:$A$124</definedName>
+    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[1]Set_up!$A$90:$A$124</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Functional KPIs'!$A$1:$J$3</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -68,7 +68,7 @@
     <t xml:space="preserve">Facings SOS</t>
   </si>
   <si>
-    <t xml:space="preserve">Pain Main Shelf, Oral Main Shelf, Respiratory Main Shelf, NRT Main Shelf</t>
+    <t xml:space="preserve">Pain Main Shelf, Oral Main Shelf, Respiratory Main Shelf, NRT Main Shelf, Other Main Shelf</t>
   </si>
   <si>
     <t xml:space="preserve">Exclude</t>
@@ -96,7 +96,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -133,12 +133,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -203,7 +197,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -244,15 +238,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -328,7 +318,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </externalLink>
@@ -342,24 +332,24 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L4" activeCellId="0" sqref="L4"/>
+      <selection pane="bottomRight" activeCell="K19" activeCellId="0" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="29.9919028340081"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="30.2064777327935"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.9595141700405"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="1" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="29.7773279352227"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1014" min="13" style="1" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="1025" min="1015" style="0" width="8.67611336032389"/>
@@ -403,7 +393,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" s="5" customFormat="true" ht="42.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="5" customFormat="true" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
@@ -429,11 +419,11 @@
       <c r="K2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
@@ -456,8 +446,8 @@
       <c r="H3" s="0"/>
       <c r="I3" s="0"/>
       <c r="J3" s="0"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="12" t="s">
+      <c r="K3" s="10"/>
+      <c r="L3" s="11" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
PROS-12731 - GSKAU Template Update Task Grocery
</commit_message>
<xml_diff>
--- a/Projects/GSKAU/Data/gsk_set_up.xlsx
+++ b/Projects/GSKAU/Data/gsk_set_up.xlsx
@@ -14,7 +14,7 @@
     <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
-    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[1]Set_up!$A$90:$A$124</definedName>
+    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[2]Set_up!$A$90:$A$124</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Functional KPIs'!$A$1:$J$3</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
   <si>
     <t xml:space="preserve">KPI Type</t>
   </si>
@@ -68,7 +68,9 @@
     <t xml:space="preserve">Facings SOS</t>
   </si>
   <si>
-    <t xml:space="preserve">Pain Main Shelf, Oral Main Shelf, Respiratory Main Shelf, NRT Main Shelf, Other Main Shelf</t>
+    <t xml:space="preserve">Pain Main Shelf, Oral Main Shelf, Respiratory Main Shelf, NRT Main Shelf, Other Main Shelf, Pain Main Shelf – Grcy,
+Oral Main Shelf – Grcy,
+NRT Main Shelf – Grcy</t>
   </si>
   <si>
     <t xml:space="preserve">Exclude</t>
@@ -81,6 +83,9 @@
   </si>
   <si>
     <t xml:space="preserve">Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pain Main Shelf, Oral Main Shelf, Respiratory Main Shelf, NRT Main Shelf, Other Main Shelf, Pain Main Shelf – Grcy, Oral Main Shelf – Grcy, NRT Main Shelf – Grcy</t>
   </si>
   <si>
     <t xml:space="preserve">Include </t>
@@ -318,7 +323,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </externalLink>
@@ -336,20 +341,20 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K19" activeCellId="0" sqref="K19"/>
+      <selection pane="bottomRight" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.9595141700405"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="55.7732793522267"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.1740890688259"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="1" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="29.9919028340081"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1014" min="13" style="1" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="1025" min="1015" style="0" width="8.67611336032389"/>
@@ -393,7 +398,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" s="5" customFormat="true" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="5" customFormat="true" ht="68.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
@@ -423,16 +428,16 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="7" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>14</v>
@@ -453,7 +458,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>

</xml_diff>

<commit_message>
GSKAU setup file scene_type hypen fix
</commit_message>
<xml_diff>
--- a/Projects/GSKAU/Data/gsk_set_up.xlsx
+++ b/Projects/GSKAU/Data/gsk_set_up.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t xml:space="preserve">KPI Type</t>
   </si>
@@ -68,9 +68,7 @@
     <t xml:space="preserve">Facings SOS</t>
   </si>
   <si>
-    <t xml:space="preserve">Pain Main Shelf, Oral Main Shelf, Respiratory Main Shelf, NRT Main Shelf, Other Main Shelf, Pain Main Shelf – Grcy,
-Oral Main Shelf – Grcy,
-NRT Main Shelf – Grcy</t>
+    <t xml:space="preserve">Pain Main Shelf, Oral Main Shelf, Respiratory Main Shelf, NRT Main Shelf, Other Main Shelf, Pain Main Shelf - Grcy, Oral Main Shelf - Grcy, NRT Main Shelf - Grcy</t>
   </si>
   <si>
     <t xml:space="preserve">Exclude</t>
@@ -83,9 +81,6 @@
   </si>
   <si>
     <t xml:space="preserve">Availability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pain Main Shelf, Oral Main Shelf, Respiratory Main Shelf, NRT Main Shelf, Other Main Shelf, Pain Main Shelf – Grcy, Oral Main Shelf – Grcy, NRT Main Shelf – Grcy</t>
   </si>
   <si>
     <t xml:space="preserve">Include </t>
@@ -341,20 +336,20 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.4939271255061"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="55.7732793522267"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="91.4453441295547"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.6032388663968"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="1" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="29.9919028340081"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="30.6356275303644"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1014" min="13" style="1" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="1025" min="1015" style="0" width="8.67611336032389"/>
@@ -398,7 +393,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" s="5" customFormat="true" ht="68.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="5" customFormat="true" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
@@ -428,16 +423,16 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>19</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>14</v>
@@ -458,10 +453,10 @@
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
+      <c r="C4" s="7"/>
       <c r="D4" s="8" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
GSKAU Wellness Main Shelf add in SOS and MSL
</commit_message>
<xml_diff>
--- a/Projects/GSKAU/Data/gsk_set_up.xlsx
+++ b/Projects/GSKAU/Data/gsk_set_up.xlsx
@@ -68,7 +68,7 @@
     <t xml:space="preserve">Facings SOS</t>
   </si>
   <si>
-    <t xml:space="preserve">Pain Main Shelf, Oral Main Shelf, Respiratory Main Shelf, NRT Main Shelf, Other Main Shelf, Pain Main Shelf - Grcy, Oral Main Shelf - Grcy, NRT Main Shelf - Grcy</t>
+    <t xml:space="preserve">Pain Main Shelf, Oral Main Shelf, Respiratory Main Shelf, NRT Main Shelf, Other Main Shelf, Pain Main Shelf - Grcy, Oral Main Shelf - Grcy, NRT Main Shelf – Grcy, Wellness Main Shelf</t>
   </si>
   <si>
     <t xml:space="preserve">Exclude</t>
@@ -336,20 +336,20 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="bottomRight" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.6032388663968"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="91.4453441295547"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="92.2307692307692"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.7085020242915"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="1" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="30.6356275303644"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="30.8502024291498"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1014" min="13" style="1" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="1025" min="1015" style="0" width="8.67611336032389"/>
@@ -423,7 +423,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
GSKAU Wellness Main Shelf-Grcy add in SOS and MSL
</commit_message>
<xml_diff>
--- a/Projects/GSKAU/Data/gsk_set_up.xlsx
+++ b/Projects/GSKAU/Data/gsk_set_up.xlsx
@@ -14,7 +14,7 @@
     <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
-    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[2]Set_up!$A$90:$A$124</definedName>
+    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[1]Set_up!$A$90:$A$124</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Functional KPIs'!$A$1:$J$3</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -68,7 +68,7 @@
     <t xml:space="preserve">Facings SOS</t>
   </si>
   <si>
-    <t xml:space="preserve">Pain Main Shelf, Oral Main Shelf, Respiratory Main Shelf, NRT Main Shelf, Other Main Shelf, Pain Main Shelf - Grcy, Oral Main Shelf - Grcy, NRT Main Shelf – Grcy, Wellness Main Shelf</t>
+    <t xml:space="preserve">Pain Main Shelf, Oral Main Shelf, Respiratory Main Shelf, NRT Main Shelf, Other Main Shelf, Pain Main Shelf - Grcy, Oral Main Shelf - Grcy, NRT Main Shelf – Grcy, Wellness Main Shelf, Wellness Main Shelf – Grcy</t>
   </si>
   <si>
     <t xml:space="preserve">Exclude</t>
@@ -318,7 +318,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </externalLink>
@@ -341,15 +341,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.7085020242915"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="92.2307692307692"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="93.085020242915"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.8178137651822"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="1" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="31.17004048583"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1014" min="13" style="1" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="1025" min="1015" style="0" width="8.67611336032389"/>

</xml_diff>

<commit_message>
Added allow-empty filter in blocking KPI
</commit_message>
<xml_diff>
--- a/Projects/GSKAU/Data/gsk_set_up.xlsx
+++ b/Projects/GSKAU/Data/gsk_set_up.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t xml:space="preserve">KPI Type</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t xml:space="preserve">Adult,Child,Topical,Osteo,Pain Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GSK_LAYOUT_COMPLIANCE_BLOCK</t>
   </si>
 </sst>
 </file>
@@ -202,7 +205,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -253,6 +256,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -336,17 +343,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="95.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="16.43"/>
@@ -356,8 +363,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="23.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="31.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1014" min="13" style="1" width="8.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1015" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1014" min="13" style="1" width="8.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1015" style="0" width="8.7"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="45.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -398,7 +405,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" s="5" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="5" customFormat="true" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
@@ -428,7 +435,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
@@ -453,7 +460,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -483,6 +490,15 @@
         <v>14</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <autoFilter ref="A1:L4"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>